<commit_message>
Modificacions en els menús. Redisseny de pantalles. Afegits nivells. Modificats scripts. Penjat esborrany de la memòria.
</commit_message>
<xml_diff>
--- a/Material/Documents/Document_SRS.xlsx
+++ b/Material/Documents/Document_SRS.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lluismasdeu/Desktop/PPROG1-P_Final/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lluismasdeu/Desktop/PPROG1/Material/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Codi de projecte:</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Lluís Masdeu</t>
   </si>
   <si>
-    <t>Programar un joc de plataformes en C#, empant el motor Unity.</t>
-  </si>
-  <si>
     <t>Joc per a escriptori de plataformes en 2D.</t>
   </si>
   <si>
@@ -120,13 +117,22 @@
   </si>
   <si>
     <t>Control d'enemics de manera autònoma.</t>
+  </si>
+  <si>
+    <t>Desenvolupar un joc de plataformes en C#, emprant el motor Unity.</t>
+  </si>
+  <si>
+    <t>NFYLS</t>
+  </si>
+  <si>
+    <t>Planetjament inicial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +143,22 @@
     <font>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -236,8 +258,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -259,26 +283,28 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -559,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:E4"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -569,21 +595,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="7" t="s">
         <v>16</v>
       </c>
@@ -597,11 +623,13 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="7"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="2" t="s">
@@ -612,10 +640,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="7" t="s">
         <v>2</v>
       </c>
@@ -623,10 +651,10 @@
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="7" t="s">
         <v>17</v>
       </c>
@@ -634,10 +662,10 @@
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="9"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="7" t="s">
         <v>18</v>
       </c>
@@ -645,10 +673,10 @@
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="9"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="7" t="s">
         <v>19</v>
       </c>
@@ -683,69 +711,71 @@
       <c r="A12" s="6">
         <v>42717</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="10">
         <v>1</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="11"/>
       <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
-      <c r="B13" s="11"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="12"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="13"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
       <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
-      <c r="B14" s="11"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="12"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="13"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
       <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
-      <c r="B15" s="11"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="12"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="13"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
       <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
-      <c r="B16" s="11"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="12"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="13"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11"/>
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
-      <c r="B17" s="11"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="12"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="13"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11"/>
       <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
-      <c r="B18" s="11"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="12"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="13"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11"/>
       <c r="G18" s="12"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -757,7 +787,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -778,7 +808,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -792,7 +822,7 @@
         <v>2</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -806,7 +836,7 @@
         <v>3</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -847,7 +877,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -860,15 +890,15 @@
       <c r="A33" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>1</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -881,7 +911,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -894,7 +924,7 @@
         <v>3</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -907,7 +937,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -1203,38 +1233,31 @@
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="B61:G61"/>
+    <mergeCell ref="B62:G62"/>
+    <mergeCell ref="B63:G63"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="B43:G43"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:B5"/>
@@ -1249,31 +1272,38 @@
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:E7"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="B43:G43"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B53:G53"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:G59"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="B61:G61"/>
-    <mergeCell ref="B62:G62"/>
-    <mergeCell ref="B63:G63"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B38:G38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>

</xml_diff>